<commit_message>
Select Random Player and fix budget calculation after each bid
</commit_message>
<xml_diff>
--- a/auction_data.xlsx
+++ b/auction_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="28">
   <si>
     <t xml:space="preserve">Participant</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Vipul</t>
+  </si>
+  <si>
+    <t>Ben Stokes</t>
+  </si>
+  <si>
+    <t>Rohit Sharma</t>
   </si>
 </sst>
 </file>
@@ -349,10 +355,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="n" s="0">
         <v>10.0</v>
@@ -360,35 +366,35 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>25.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>10.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -523,7 +529,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>100.0</v>
+        <v>85.0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added Base Price on the board
</commit_message>
<xml_diff>
--- a/auction_data.xlsx
+++ b/auction_data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="28">
   <si>
     <t xml:space="preserve">Participant</t>
   </si>
@@ -330,7 +330,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
@@ -351,50 +351,6 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C3" t="n" s="0">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +477,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,7 +485,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>85.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>